<commit_message>
Add empty arr example Self review
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C23C57-FB73-4DF5-9B3F-222DDCD487E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CA7539-66C3-40CB-B1E7-8B105A2AEA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lvl0" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
   <si>
     <t>season</t>
   </si>
@@ -117,6 +117,24 @@
   </si>
   <si>
     <t>arr</t>
+  </si>
+  <si>
+    <t>seasonEmptyArr</t>
+  </si>
+  <si>
+    <t>field6</t>
+  </si>
+  <si>
+    <t>seasonArrWithEmptyItems</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ref </t>
+  </si>
+  <si>
+    <t>seasonArrWithEmptyItems_item1</t>
+  </si>
+  <si>
+    <t>seasonArrWithEmptyItems_item2</t>
   </si>
 </sst>
 </file>
@@ -465,13 +483,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
-  <dimension ref="B1:F19"/>
+  <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
@@ -564,22 +585,44 @@
         <v>22</v>
       </c>
     </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" t="s">
+        <v>30</v>
+      </c>
+    </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18">
+      <c r="D18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25">
         <v>123</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>19</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D26" t="s">
         <v>6</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E26" t="s">
         <v>26</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F26" t="s">
         <v>20</v>
       </c>
     </row>
@@ -591,15 +634,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881CF64C-A86A-443D-BF50-D39123249C40}">
-  <dimension ref="B1:F14"/>
+  <dimension ref="B1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F20" sqref="F20:F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -681,6 +724,30 @@
       </c>
       <c r="F14" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -690,15 +757,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF7E211-A32D-4C6F-A0D1-E6C04CAD2CBB}">
-  <dimension ref="B1:F12"/>
+  <dimension ref="B1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="3" max="3" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -768,6 +835,16 @@
         <v>123</v>
       </c>
     </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix errors unknown types
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CA7539-66C3-40CB-B1E7-8B105A2AEA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCE25F-E754-449F-8970-FCCF339C86C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lvl0" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
   <si>
     <t>season</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t>seasonArrWithEmptyItems</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ref </t>
   </si>
   <si>
     <t>seasonArrWithEmptyItems_item1</t>
@@ -485,7 +482,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -636,8 +633,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881CF64C-A86A-443D-BF50-D39123249C40}">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20:F21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,18 +733,18 @@
         <v>32</v>
       </c>
       <c r="E20" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" t="s">
         <v>33</v>
-      </c>
-      <c r="F20" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="F21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -837,12 +834,12 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add example: empty object
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BFCE25F-E754-449F-8970-FCCF339C86C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0D3E762-2DD6-4F17-8CD9-70DE7502E34A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="37">
   <si>
     <t>season</t>
   </si>
@@ -132,6 +132,12 @@
   </si>
   <si>
     <t>seasonArrWithEmptyItems_item2</t>
+  </si>
+  <si>
+    <t>field7</t>
+  </si>
+  <si>
+    <t>seasonEmptyField</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
   <dimension ref="B1:F26"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +610,17 @@
         <v>32</v>
       </c>
     </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>123</v>
@@ -631,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881CF64C-A86A-443D-BF50-D39123249C40}">
-  <dimension ref="B1:F21"/>
+  <dimension ref="B1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,6 +762,11 @@
       </c>
       <c r="F21" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added truncate empty spaces
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEDAC6C-8CD5-4532-A02E-DD118ACB3FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AA8F4A-37D3-4FB8-8458-980C49D3FD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
   <si>
     <t>season</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>seasonDict_item2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">field2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> field3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   str</t>
   </si>
 </sst>
 </file>
@@ -845,7 +854,7 @@
   <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,7 +895,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="E8" t="s">
         <v>27</v>
@@ -900,10 +909,10 @@
         <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Added start parse at row index. Replaced any value type in ignore field on only bool type (available value: empty, "true", "false", "1", "0"). If type is incorrect printed warning
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57AA8F4A-37D3-4FB8-8458-980C49D3FD3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D014EF8-C6E9-417F-BD50-0733458A91A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lvl0" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
   <si>
     <t>season</t>
   </si>
@@ -50,9 +50,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>qw</t>
-  </si>
-  <si>
     <t>fiel1</t>
   </si>
   <si>
@@ -165,6 +162,12 @@
   </si>
   <si>
     <t xml:space="preserve">   str</t>
+  </si>
+  <si>
+    <t>ignoredFeature2</t>
+  </si>
+  <si>
+    <t>ignoredFeature1</t>
   </si>
 </sst>
 </file>
@@ -516,12 +519,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -542,9 +546,20 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="b">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>7</v>
+      <c r="B10" t="b">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -555,18 +570,18 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>10</v>
@@ -577,106 +592,109 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>28</v>
+      </c>
+      <c r="F15" t="s">
         <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F15" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
         <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F17" t="s">
         <v>29</v>
-      </c>
-      <c r="F17" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
         <v>31</v>
-      </c>
-      <c r="E18" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" t="s">
         <v>35</v>
-      </c>
-      <c r="E19" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
         <v>37</v>
       </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>123</v>
+      <c r="B25" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="b">
+        <v>0</v>
+      </c>
       <c r="C26" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" t="s">
         <v>6</v>
       </c>
       <c r="E26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -718,16 +736,16 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -735,91 +753,91 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" t="s">
         <v>16</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" t="s">
         <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" t="s">
         <v>32</v>
-      </c>
-      <c r="E20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>37</v>
+      </c>
+      <c r="D25" t="s">
         <v>38</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
@@ -827,10 +845,10 @@
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.25">
@@ -838,10 +856,10 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -853,7 +871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EF7E211-A32D-4C6F-A0D1-E6C04CAD2CBB}">
   <dimension ref="B1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -881,24 +899,24 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F8">
         <v>123</v>
@@ -906,24 +924,24 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" t="s">
         <v>24</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12">
         <v>123</v>
@@ -931,37 +949,37 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F19">
         <v>456</v>

</xml_diff>

<commit_message>
Refactor. RowToJsonConverter: Added highlite error type in row parse
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D014EF8-C6E9-417F-BD50-0733458A91A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E15E0C-2C20-4107-98B3-62124E878426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,7 +520,7 @@
   <dimension ref="B1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor: Add print missing ref value
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6E15E0C-2C20-4107-98B3-62124E878426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281378B-9129-4525-A730-84A61D3C4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lvl0" sheetId="5" r:id="rId1"/>
@@ -519,7 +519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -707,8 +707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881CF64C-A86A-443D-BF50-D39123249C40}">
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Refactor: Add print missing ref value after shet names ended
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E281378B-9129-4525-A730-84A61D3C4633}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6142056-C6BA-4E3F-992B-FB5028B1A362}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lvl0" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="48">
   <si>
     <t>season</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>ignoredFeature1</t>
+  </si>
+  <si>
+    <t>field41</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +566,9 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="b">
+        <v>0</v>
+      </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
@@ -611,7 +617,7 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>14</v>
+        <v>47</v>
       </c>
       <c r="E15" t="s">
         <v>28</v>
@@ -707,7 +713,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881CF64C-A86A-443D-BF50-D39123249C40}">
   <dimension ref="B1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -872,7 +878,7 @@
   <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added support Google Sheets
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DAFD39-1A47-4084-9562-AF5BE7A60DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90E37CC-C092-40F8-A565-6DF69F55DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -849,7 +849,7 @@
   <dimension ref="B1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14:G14"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,7 +865,7 @@
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Added feature: Json alias funcs
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Parser2\Example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Repo\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90E37CC-C092-40F8-A565-6DF69F55DDCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0D5057-F8E0-42D4-813E-14424FFA8F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7125" yWindow="480" windowWidth="16800" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AliasFuncsLvl0" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="85">
   <si>
     <t>season</t>
   </si>
@@ -645,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF3775B-0503-476A-AAFE-9E00D6710E21}">
-  <dimension ref="B1:G17"/>
+  <dimension ref="B1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,154 +679,140 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D5" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D5" t="s">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F6" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>56</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D7" t="s">
         <v>38</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D7" t="s">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
         <v>51</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
-        <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>10</v>
       </c>
       <c r="E8" t="s">
         <v>26</v>
       </c>
       <c r="F8" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
       <c r="D9" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E9" t="s">
         <v>26</v>
       </c>
       <c r="F9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>64</v>
-      </c>
       <c r="D10" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
         <v>26</v>
       </c>
       <c r="F10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>64</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>56</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>51</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
         <v>66</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>10</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E13" t="s">
         <v>27</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F13" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
         <v>72</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>10</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E15" t="s">
         <v>27</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F15" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="17" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -835,6 +821,20 @@
         <v>27</v>
       </c>
       <c r="F17" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" t="s">
         <v>82</v>
       </c>
     </row>
@@ -846,10 +846,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59DC35DD-449B-417F-A9B5-07ABDEE8B4C2}">
-  <dimension ref="B1:G14"/>
+  <dimension ref="B1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -964,14 +964,6 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="F14" t="s">
-        <v>51</v>
-      </c>
-      <c r="G14" t="s">
-        <v>80</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -979,11 +971,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
-  <dimension ref="B1:G39"/>
+  <dimension ref="B1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,91 +1210,75 @@
         <v>500</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F28" t="s">
-        <v>51</v>
-      </c>
-      <c r="G28">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="F29" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29">
-        <v>12324</v>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>71</v>
+      </c>
+      <c r="E30" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>72</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E34" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>75</v>
-      </c>
-      <c r="G34" t="s">
-        <v>24</v>
+        <v>51</v>
+      </c>
+      <c r="G34">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35">
+        <v>2000</v>
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
-        <v>79</v>
-      </c>
-      <c r="E36" t="s">
-        <v>77</v>
-      </c>
-      <c r="F36" t="s">
-        <v>51</v>
-      </c>
-      <c r="G36">
-        <v>1500</v>
+      <c r="B36" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B37" t="b">
+        <v>0</v>
+      </c>
+      <c r="C37" t="s">
+        <v>18</v>
+      </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="E37" t="s">
-        <v>81</v>
+        <v>25</v>
       </c>
       <c r="F37" t="s">
-        <v>84</v>
-      </c>
-      <c r="G37">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B38" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B39" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>25</v>
-      </c>
-      <c r="F39" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1316,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{881CF64C-A86A-443D-BF50-D39123249C40}">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Aded feature: Anonym args for alias funcs
</commit_message>
<xml_diff>
--- a/Parser2/Example/Doc.xlsx
+++ b/Parser2/Example/Doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFolder\Projects\ExcelToJsonUniversalParser\Repo\Parser2\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B0D5057-F8E0-42D4-813E-14424FFA8F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{854A2F40-D345-418B-8159-F09AAE05A642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7125" yWindow="480" windowWidth="16800" windowHeight="11055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AliasFuncsLvl0" sheetId="6" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="95">
   <si>
     <t>season</t>
   </si>
@@ -284,6 +284,36 @@
   </si>
   <si>
     <t>wrap_amount_arg</t>
+  </si>
+  <si>
+    <t>field18</t>
+  </si>
+  <si>
+    <t>arg3</t>
+  </si>
+  <si>
+    <t>HardGoodWithAnonymArg</t>
+  </si>
+  <si>
+    <t>workaround for float type</t>
+  </si>
+  <si>
+    <t>amount1</t>
+  </si>
+  <si>
+    <t>%arg3%</t>
+  </si>
+  <si>
+    <t>field19</t>
+  </si>
+  <si>
+    <t>ExampleExcelAliasFuncWithAnonymArg1</t>
+  </si>
+  <si>
+    <t>ExampleExcelAliasFuncWithAnonymArg2</t>
+  </si>
+  <si>
+    <t>field20</t>
   </si>
 </sst>
 </file>
@@ -356,13 +386,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -645,21 +685,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF3775B-0503-476A-AAFE-9E00D6710E21}">
-  <dimension ref="B1:G18"/>
+  <dimension ref="B1:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" customWidth="1"/>
     <col min="6" max="6" width="61" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -678,8 +718,17 @@
       <c r="G1" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>49</v>
       </c>
@@ -693,7 +742,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D6" t="s">
         <v>51</v>
       </c>
@@ -704,7 +753,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>56</v>
       </c>
@@ -718,7 +767,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>51</v>
       </c>
@@ -729,7 +778,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>58</v>
       </c>
@@ -743,7 +792,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D10" t="s">
         <v>1</v>
       </c>
@@ -754,7 +803,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
         <v>64</v>
       </c>
@@ -768,7 +817,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>1</v>
       </c>
@@ -782,7 +831,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
         <v>66</v>
       </c>
@@ -796,7 +845,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>72</v>
       </c>
@@ -810,7 +859,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
         <v>77</v>
       </c>
@@ -824,7 +873,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
         <v>81</v>
       </c>
@@ -836,11 +885,79 @@
       </c>
       <c r="F18" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>93</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>92</v>
+      </c>
+      <c r="H25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I25" t="s">
+        <v>60</v>
+      </c>
+      <c r="J25" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -971,11 +1088,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A34CEDD6-A5B9-4B80-94E2-5A256F041AA6}">
-  <dimension ref="B1:G37"/>
+  <dimension ref="B1:J42"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="A38:XFD39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,9 +1101,12 @@
     <col min="5" max="5" width="43.85546875" customWidth="1"/>
     <col min="6" max="6" width="28.5703125" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" style="4" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -1005,8 +1125,28 @@
       <c r="G1" s="3" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="2:10" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="b">
         <v>1</v>
       </c>
@@ -1014,7 +1154,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="b">
         <v>1</v>
       </c>
@@ -1022,7 +1162,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="b">
         <v>0</v>
       </c>
@@ -1039,7 +1179,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D12" t="s">
         <v>7</v>
       </c>
@@ -1050,7 +1190,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D13" t="s">
         <v>1</v>
       </c>
@@ -1061,7 +1201,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>13</v>
       </c>
@@ -1072,7 +1212,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
         <v>47</v>
       </c>
@@ -1083,7 +1223,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
         <v>20</v>
       </c>
@@ -1232,7 +1372,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D34" t="s">
         <v>79</v>
       </c>
@@ -1246,7 +1386,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="D35" t="s">
         <v>83</v>
       </c>
@@ -1260,31 +1400,97 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B36" t="b">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>85</v>
+      </c>
+      <c r="E36" t="s">
+        <v>87</v>
+      </c>
+      <c r="F36" t="s">
+        <v>51</v>
+      </c>
+      <c r="G36">
+        <v>1000</v>
+      </c>
+      <c r="H36" s="4">
+        <v>123</v>
+      </c>
+      <c r="I36" s="4">
+        <v>1234</v>
+      </c>
+      <c r="J36" s="4">
+        <v>12345</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" t="s">
+        <v>92</v>
+      </c>
+      <c r="H38" s="4">
+        <v>321</v>
+      </c>
+      <c r="I38" s="4">
+        <v>4321</v>
+      </c>
+      <c r="J38" s="4">
+        <v>54321</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>94</v>
+      </c>
+      <c r="E39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H39" s="4">
+        <v>987</v>
+      </c>
+      <c r="I39" s="4">
+        <v>9876</v>
+      </c>
+      <c r="J39" s="4">
+        <v>98765</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B37" t="b">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" t="b">
         <v>0</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C42" t="s">
         <v>18</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D42" t="s">
         <v>6</v>
       </c>
-      <c r="E37" t="s">
+      <c r="E42" t="s">
         <v>25</v>
       </c>
-      <c r="F37" t="s">
+      <c r="F42" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>